<commit_message>
Timesheet Update für LV Einheit
</commit_message>
<xml_diff>
--- a/docs/Timesheets/Timesheet-Georg-Wenzel.xlsx
+++ b/docs/Timesheets/Timesheet-Georg-Wenzel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7774CA9A-4AD5-444D-8F16-740720559F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE20DF35-AF0E-40A6-9083-346934AA4BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
   <si>
     <t>Datum</t>
   </si>
@@ -240,6 +240,42 @@
   </si>
   <si>
     <t>Redesign/Rework Dice Side Config. (Frontend)</t>
+  </si>
+  <si>
+    <t>Bugfixes</t>
+  </si>
+  <si>
+    <t>Fixes für Tabellen und Filtermöglichkeiten</t>
+  </si>
+  <si>
+    <t>Booking Test Coverage</t>
+  </si>
+  <si>
+    <t>Bookings Test Coverage</t>
+  </si>
+  <si>
+    <t>Implementierung Statistik Views</t>
+  </si>
+  <si>
+    <t>Test Coverage</t>
+  </si>
+  <si>
+    <t>Softwarekonzept &amp; Testdrehbuch</t>
+  </si>
+  <si>
+    <t>Besprechung, Softwarekonzept</t>
+  </si>
+  <si>
+    <t>Einarbeitung fremdes Testsystem</t>
+  </si>
+  <si>
+    <t>Testdurchführung, Dokumentation</t>
+  </si>
+  <si>
+    <t>Abnahmeetst Dokument finalisieren.</t>
+  </si>
+  <si>
+    <t>Testcoverage</t>
   </si>
 </sst>
 </file>
@@ -668,10 +704,10 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N45" sqref="N45"/>
+      <selection pane="bottomRight" activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1579,88 +1615,298 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="6"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="6">
+        <v>43969</v>
+      </c>
+      <c r="B65" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="6">
+        <v>43969</v>
+      </c>
+      <c r="B66" s="9">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="6"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="6">
+        <v>43970</v>
+      </c>
+      <c r="B67" s="9">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="6"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="6">
+        <v>43972</v>
+      </c>
+      <c r="B68" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="6">
+        <v>43972</v>
+      </c>
+      <c r="B69" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="6">
+        <v>43973</v>
+      </c>
+      <c r="B70" s="9">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="6"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="6">
+        <v>43973</v>
+      </c>
+      <c r="B71" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="6"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="6">
+        <v>43974</v>
+      </c>
+      <c r="B72" s="9">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="6"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="6">
+        <v>43975</v>
+      </c>
+      <c r="B73" s="9">
+        <v>9.375E-2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="6"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="6">
+        <v>43976</v>
+      </c>
+      <c r="B74" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="6"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="6">
+        <v>43976</v>
+      </c>
+      <c r="B75" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="6"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="6">
+        <v>43977</v>
+      </c>
+      <c r="B76" s="9">
+        <v>0.15625</v>
+      </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="6"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="6">
+        <v>43978</v>
+      </c>
+      <c r="B77" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="6"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="6">
+        <v>43979</v>
+      </c>
+      <c r="B78" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="6"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="6">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="6"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="6">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="6"/>
-      <c r="D81" s="3"/>
+      <c r="A81" s="6">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="6"/>
-      <c r="D82" s="3"/>
+      <c r="A82" s="6">
+        <v>43983</v>
+      </c>
+      <c r="B82" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="6"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="6">
+        <v>43985</v>
+      </c>
+      <c r="B83" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="6"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="6">
+        <v>43987</v>
+      </c>
+      <c r="B84" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="6"/>
-      <c r="D85" s="3"/>
+      <c r="A85" s="6">
+        <v>43988</v>
+      </c>
+      <c r="B85" s="9">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="6"/>

</xml_diff>